<commit_message>
update xls template + scoreboard filter fix
</commit_message>
<xml_diff>
--- a/public/files/excel/waterpolo_template.xlsx
+++ b/public/files/excel/waterpolo_template.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>name</t>
   </si>
@@ -34,6 +34,12 @@
   </si>
   <si>
     <t>status</t>
+  </si>
+  <si>
+    <t>Testplayer</t>
+  </si>
+  <si>
+    <t>Testplayer2</t>
   </si>
 </sst>
 </file>
@@ -355,11 +361,12 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="15.44140625" customWidth="1"/>
     <col min="2" max="2" width="17.109375" customWidth="1"/>
     <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -382,10 +389,38 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C2" s="1"/>
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>55</v>
+      </c>
+      <c r="C2" s="1">
+        <v>37194.833333333336</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C3" s="1"/>
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>56</v>
+      </c>
+      <c r="C3" s="1">
+        <v>37340.333333333336</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>